<commit_message>
rearrange data table, metadata updates
</commit_message>
<xml_diff>
--- a/trawl-transect-info.xlsx
+++ b/trawl-transect-info.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="144">
   <si>
     <t>attributeName</t>
   </si>
@@ -116,9 +116,6 @@
     <t>definition</t>
   </si>
   <si>
-    <t>categorical</t>
-  </si>
-  <si>
     <t>PI</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>abundance</t>
   </si>
   <si>
-    <t>eventID</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -233,24 +227,12 @@
     <t>Aphia ID</t>
   </si>
   <si>
-    <t>individualCount</t>
-  </si>
-  <si>
     <t>split</t>
   </si>
   <si>
-    <t>Abundant taxa were counted from a split</t>
-  </si>
-  <si>
     <t>Trawl number sequential within cruise</t>
   </si>
   <si>
-    <t>The number of vessels the sample was put into</t>
-  </si>
-  <si>
-    <t>Which of the sampling jars was processed</t>
-  </si>
-  <si>
     <t>eventDate</t>
   </si>
   <si>
@@ -332,9 +314,6 @@
     <t>preparations</t>
   </si>
   <si>
-    <t>Substance and/or method of preservation of each sample, typically formalin or ethanol </t>
-  </si>
-  <si>
     <t>YYYY-MM-DD</t>
   </si>
   <si>
@@ -371,9 +350,6 @@
     <t>depth_tow</t>
   </si>
   <si>
-    <t>Identifier consisting of cruise identifier and cast http://rs.tdwg.org/dwc/terms/eventID</t>
-  </si>
-  <si>
     <t>Family name of taxon http://rs.tdwg.org/dwc/terms/family</t>
   </si>
   <si>
@@ -383,24 +359,12 @@
     <t>Taxon scientific name identifier http://rs.tdwg.org/dwc/terms/scientificNameID</t>
   </si>
   <si>
-    <t>Taxon life stage http://rs.tdwg.org/dwc/iri/lifeStage</t>
-  </si>
-  <si>
     <t>Taxon descriptive name  http://rs.tdwg.org/dwc/terms/verbatimIdentification</t>
   </si>
   <si>
-    <t>Trawl number, chronological per cruise, corresponding to cast in ship's event log</t>
-  </si>
-  <si>
-    <t>Taxon abundance as net total http://rs.tdwg.org/dwc/terms/individualCount</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>"NA"</t>
-  </si>
-  <si>
     <t xml:space="preserve">event </t>
   </si>
   <si>
@@ -413,9 +377,6 @@
     <t>Depth of the tow in meters; if a range, deployment was a towyo http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
     <t>no_of_jars</t>
   </si>
   <si>
@@ -423,6 +384,54 @@
   </si>
   <si>
     <t>Time in UTC when the trawl net exited the water column</t>
+  </si>
+  <si>
+    <t>HRS2303_1</t>
+  </si>
+  <si>
+    <t>HRS2303_2</t>
+  </si>
+  <si>
+    <t>HRS2303_3</t>
+  </si>
+  <si>
+    <t>EN706_1</t>
+  </si>
+  <si>
+    <t>EN706_2</t>
+  </si>
+  <si>
+    <t>EN706_3</t>
+  </si>
+  <si>
+    <t>AR77_3</t>
+  </si>
+  <si>
+    <t>AR77_4</t>
+  </si>
+  <si>
+    <t>AR77_5</t>
+  </si>
+  <si>
+    <t>The number of sample vessels preserved from the catch</t>
+  </si>
+  <si>
+    <t>Identification number of sample vessel processed for identification and counting</t>
+  </si>
+  <si>
+    <t>Substance and/or method of preservation of each sample, typically formalin or ethanol https://dwc.tdwg.org/list/#dwc_preparations</t>
+  </si>
+  <si>
+    <t>Taxon life stage http://rs.tdwg.org/dwc/iri/lifeStage using BODC vocabulary http://vocab.nerc.ac.uk/collection/S11/current/</t>
+  </si>
+  <si>
+    <t>Taxon abundance as total number of individuals caught in trawl net from event corresponding to column name</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Not taxonomically identified</t>
   </si>
 </sst>
 </file>
</xml_diff>